<commit_message>
update views, utils, bbdd
</commit_message>
<xml_diff>
--- a/bbdd_project.xlsx
+++ b/bbdd_project.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lordtuestaperington/Desktop/The Bridge Bootcamp/data-bridge/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/auxi/data-bridge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D38E432-EB77-1542-A66D-F21920D6B2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA8F4CC-D3D5-D94F-B5AA-9022480DF02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{5EDA1284-4A66-5F48-AB6E-D39D2757404B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" activeTab="1" xr2:uid="{5EDA1284-4A66-5F48-AB6E-D39D2757404B}"/>
   </bookViews>
   <sheets>
     <sheet name="formularios" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="71">
   <si>
     <t>employee_id</t>
   </si>
@@ -67,15 +67,6 @@
     <t>yan sa</t>
   </si>
   <si>
-    <t>paco sa</t>
-  </si>
-  <si>
-    <t>david sa</t>
-  </si>
-  <si>
-    <t>esteban sa</t>
-  </si>
-  <si>
     <t>¿Ha establecido su empresa un diálogo con los grupos o partes interesadas en materia de sostenibilidad?</t>
   </si>
   <si>
@@ -257,6 +248,9 @@
   </si>
   <si>
     <t>type_response_id</t>
+  </si>
+  <si>
+    <t>¿Forma parte de alguna alianza/organización/asociación de promoción de la sostenibilidad?</t>
   </si>
 </sst>
 </file>
@@ -313,7 +307,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,12 +318,6 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -347,12 +335,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -449,24 +431,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -474,23 +455,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -498,17 +476,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -823,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7D95FDC-1C2C-7C46-8223-B3D0A8CB6EF2}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView zoomScale="92" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -849,7 +830,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -866,7 +847,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -900,7 +881,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -918,7 +899,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -935,7 +916,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -969,7 +950,7 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -986,7 +967,7 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1003,7 +984,7 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1037,7 +1018,7 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1054,7 +1035,7 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1071,7 +1052,7 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1105,7 +1086,7 @@
         <v>15</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1122,7 +1103,7 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1139,7 +1120,7 @@
         <v>17</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1173,7 +1154,7 @@
         <v>19</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1190,7 +1171,7 @@
         <v>20</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1207,7 +1188,7 @@
         <v>21</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1240,7 +1221,7 @@
       <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24" s="41">
+      <c r="C24" s="36">
         <v>0</v>
       </c>
       <c r="D24">
@@ -1257,7 +1238,7 @@
       <c r="B25">
         <v>2</v>
       </c>
-      <c r="C25" s="41">
+      <c r="C25" s="36">
         <v>1</v>
       </c>
       <c r="D25">
@@ -1274,8 +1255,8 @@
       <c r="B26">
         <v>3</v>
       </c>
-      <c r="C26" s="41">
-        <v>2</v>
+      <c r="C26" s="36">
+        <v>0</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -1291,8 +1272,8 @@
       <c r="B27">
         <v>4</v>
       </c>
-      <c r="C27" s="41">
-        <v>3</v>
+      <c r="C27" s="36">
+        <v>1</v>
       </c>
       <c r="D27">
         <v>3</v>
@@ -1309,7 +1290,7 @@
         <v>5</v>
       </c>
       <c r="C28">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D28">
         <v>3</v>
@@ -1325,8 +1306,8 @@
       <c r="B29">
         <v>6</v>
       </c>
-      <c r="C29" s="41">
-        <v>1</v>
+      <c r="C29" s="36">
+        <v>0</v>
       </c>
       <c r="D29">
         <v>3</v>
@@ -1342,8 +1323,8 @@
       <c r="B30">
         <v>7</v>
       </c>
-      <c r="C30" s="41">
-        <v>2</v>
+      <c r="C30" s="36">
+        <v>0</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -1359,8 +1340,8 @@
       <c r="B31">
         <v>8</v>
       </c>
-      <c r="C31" s="41">
-        <v>3</v>
+      <c r="C31" s="36">
+        <v>1</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -1377,7 +1358,7 @@
         <v>9</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D32">
         <v>3</v>
@@ -1393,7 +1374,7 @@
       <c r="B33">
         <v>10</v>
       </c>
-      <c r="C33" s="41">
+      <c r="C33" s="36">
         <v>1</v>
       </c>
       <c r="D33">
@@ -1410,8 +1391,8 @@
       <c r="B34">
         <v>11</v>
       </c>
-      <c r="C34" s="41">
-        <v>2</v>
+      <c r="C34" s="36">
+        <v>1</v>
       </c>
       <c r="D34">
         <v>3</v>
@@ -1427,8 +1408,8 @@
       <c r="B35">
         <v>12</v>
       </c>
-      <c r="C35" s="41">
-        <v>3</v>
+      <c r="C35" s="36">
+        <v>0</v>
       </c>
       <c r="D35">
         <v>3</v>
@@ -1445,7 +1426,7 @@
         <v>13</v>
       </c>
       <c r="C36">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D36">
         <v>3</v>
@@ -1461,8 +1442,8 @@
       <c r="B37">
         <v>14</v>
       </c>
-      <c r="C37" s="41">
-        <v>1</v>
+      <c r="C37" s="36">
+        <v>0</v>
       </c>
       <c r="D37">
         <v>3</v>
@@ -1478,8 +1459,8 @@
       <c r="B38">
         <v>15</v>
       </c>
-      <c r="C38" s="41">
-        <v>2</v>
+      <c r="C38" s="36">
+        <v>1</v>
       </c>
       <c r="D38">
         <v>3</v>
@@ -1495,8 +1476,8 @@
       <c r="B39">
         <v>16</v>
       </c>
-      <c r="C39" s="41">
-        <v>3</v>
+      <c r="C39" s="36">
+        <v>1</v>
       </c>
       <c r="D39">
         <v>3</v>
@@ -1513,7 +1494,7 @@
         <v>17</v>
       </c>
       <c r="C40">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D40">
         <v>3</v>
@@ -1529,7 +1510,7 @@
       <c r="B41">
         <v>18</v>
       </c>
-      <c r="C41" s="41">
+      <c r="C41" s="36">
         <v>1</v>
       </c>
       <c r="D41">
@@ -1546,8 +1527,8 @@
       <c r="B42">
         <v>19</v>
       </c>
-      <c r="C42" s="41">
-        <v>2</v>
+      <c r="C42" s="36">
+        <v>1</v>
       </c>
       <c r="D42">
         <v>3</v>
@@ -1563,8 +1544,8 @@
       <c r="B43">
         <v>20</v>
       </c>
-      <c r="C43" s="41">
-        <v>3</v>
+      <c r="C43" s="36">
+        <v>1</v>
       </c>
       <c r="D43">
         <v>3</v>
@@ -1581,7 +1562,7 @@
         <v>21</v>
       </c>
       <c r="C44">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D44">
         <v>3</v>
@@ -1604,6 +1585,380 @@
         <v>3</v>
       </c>
       <c r="E45" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" s="36">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" s="36">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48" s="36">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49" s="36">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="C50" s="36">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>6</v>
+      </c>
+      <c r="C51" s="36">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="E51" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>7</v>
+      </c>
+      <c r="C52" s="36">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>8</v>
+      </c>
+      <c r="C53" s="36">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
+      <c r="E53" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>9</v>
+      </c>
+      <c r="C54" s="36">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>10</v>
+      </c>
+      <c r="C55" s="36">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56">
+        <v>11</v>
+      </c>
+      <c r="C56" s="36">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>12</v>
+      </c>
+      <c r="C57" s="36">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <v>13</v>
+      </c>
+      <c r="C58" s="36">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>14</v>
+      </c>
+      <c r="C59" s="36">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>15</v>
+      </c>
+      <c r="C60" s="36">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>16</v>
+      </c>
+      <c r="C61" s="36">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>17</v>
+      </c>
+      <c r="C62" s="36">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>18</v>
+      </c>
+      <c r="C63" s="36">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>19</v>
+      </c>
+      <c r="C64" s="36">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65">
+        <v>20</v>
+      </c>
+      <c r="C65" s="36">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66">
+        <v>21</v>
+      </c>
+      <c r="C66" s="36">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+      <c r="E66" s="1">
+        <v>43224.855567129627</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>1</v>
+      </c>
+      <c r="B67">
+        <v>22</v>
+      </c>
+      <c r="C67" s="36">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67" s="1">
         <v>43224.855567129627</v>
       </c>
     </row>
@@ -1616,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8A0A99E-EF21-1848-9598-0B90E74EE7E1}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="108" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1634,22 +1989,22 @@
         <v>1</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>28</v>
+        <v>36</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>25</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1657,21 +2012,21 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="14">
-        <v>7.8</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>31</v>
+        <v>10</v>
+      </c>
+      <c r="D2" s="26">
+        <v>6.2</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="16">
+        <v>22</v>
+      </c>
+      <c r="G2" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1680,67 +2035,67 @@
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="26">
+        <v>6.2</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>1</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="14">
-        <v>6.3</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
-        <v>1</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="29">
+      <c r="D4" s="25">
         <v>6.2</v>
       </c>
-      <c r="E4" s="21" t="s">
-        <v>31</v>
+      <c r="E4" s="19" t="s">
+        <v>28</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="22">
+        <v>22</v>
+      </c>
+      <c r="G4" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23">
-        <v>2</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>16</v>
+      <c r="A5" s="21">
+        <v>2</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="25">
-        <v>5</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>31</v>
+        <v>10</v>
+      </c>
+      <c r="D5" s="27">
+        <v>8.4</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="27">
+        <v>23</v>
+      </c>
+      <c r="G5" s="24">
         <v>1</v>
       </c>
     </row>
@@ -1749,67 +2104,67 @@
         <v>2</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="14">
-        <v>9</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>31</v>
+        <v>11</v>
+      </c>
+      <c r="D6" s="26">
+        <v>5.22</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="16">
+        <v>23</v>
+      </c>
+      <c r="G6" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
-        <v>2</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="20">
-        <v>6.5</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>31</v>
+      <c r="A7" s="16">
+        <v>2</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="25">
+        <v>6.6</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>28</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="22">
+        <v>23</v>
+      </c>
+      <c r="G7" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23">
-        <v>3</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>17</v>
+      <c r="A8" s="21">
+        <v>3</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>70</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="25">
-        <v>7</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>31</v>
+        <v>10</v>
+      </c>
+      <c r="D8" s="27">
+        <v>7.7</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="27">
+        <v>20</v>
+      </c>
+      <c r="G8" s="24">
         <v>1</v>
       </c>
     </row>
@@ -1817,45 +2172,45 @@
       <c r="A9" s="11">
         <v>3</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>17</v>
+      <c r="B9" s="40" t="s">
+        <v>70</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="14">
-        <v>5</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>31</v>
+        <v>11</v>
+      </c>
+      <c r="D9" s="26">
+        <v>7.7</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="16">
+        <v>20</v>
+      </c>
+      <c r="G9" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
-        <v>3</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="20">
-        <v>6</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>31</v>
+      <c r="A10" s="16">
+        <v>3</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="25">
+        <v>7.7</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>28</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="22">
+        <v>20</v>
+      </c>
+      <c r="G10" s="20">
         <v>1</v>
       </c>
     </row>
@@ -1864,67 +2219,67 @@
         <v>4</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="30">
+        <v>50</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="26">
         <v>6.3</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>31</v>
+      <c r="E11" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="21">
+        <v>5</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="27">
+        <v>7.1</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23">
-        <v>5</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="31">
-        <v>7.1</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="27">
+      <c r="G12" s="24">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23">
+      <c r="A13" s="21">
         <v>6</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="31">
+      <c r="B13" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="27">
         <v>8.8000000000000007</v>
       </c>
-      <c r="E13" s="26" t="s">
-        <v>31</v>
+      <c r="E13" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="27">
+        <v>20</v>
+      </c>
+      <c r="G13" s="24">
         <v>4</v>
       </c>
     </row>
@@ -1933,67 +2288,67 @@
         <v>6</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="30">
+        <v>52</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="26">
         <v>7.4</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>31</v>
+      <c r="E14" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="16">
+        <v>20</v>
+      </c>
+      <c r="G14" s="15">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
+      <c r="A15" s="16">
         <v>6</v>
       </c>
-      <c r="B15" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="28">
+      <c r="B15" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="25">
         <v>8</v>
       </c>
-      <c r="E15" s="21" t="s">
-        <v>31</v>
+      <c r="E15" s="19" t="s">
+        <v>28</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="22">
+        <v>20</v>
+      </c>
+      <c r="G15" s="20">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23">
+      <c r="A16" s="21">
         <v>7</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="31">
+      <c r="B16" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="27">
         <v>7.2</v>
       </c>
-      <c r="E16" s="26" t="s">
-        <v>31</v>
+      <c r="E16" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="27">
+        <v>20</v>
+      </c>
+      <c r="G16" s="24">
         <v>4</v>
       </c>
     </row>
@@ -2002,67 +2357,67 @@
         <v>7</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="30">
+        <v>53</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="26">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E17" s="15" t="s">
-        <v>31</v>
+      <c r="E17" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="16">
+        <v>20</v>
+      </c>
+      <c r="G17" s="15">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
+      <c r="A18" s="16">
         <v>7</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="28">
+      <c r="B18" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="25">
         <v>6.6</v>
       </c>
-      <c r="E18" s="21" t="s">
-        <v>31</v>
+      <c r="E18" s="19" t="s">
+        <v>28</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="22">
+        <v>20</v>
+      </c>
+      <c r="G18" s="20">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="23">
+      <c r="A19" s="21">
         <v>8</v>
       </c>
-      <c r="B19" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="31">
+      <c r="B19" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="27">
         <v>2.38</v>
       </c>
-      <c r="E19" s="26" t="s">
-        <v>31</v>
+      <c r="E19" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="27">
+        <v>22</v>
+      </c>
+      <c r="G19" s="24">
         <v>5</v>
       </c>
     </row>
@@ -2071,44 +2426,44 @@
         <v>8</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="30">
+        <v>54</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="26">
         <v>1.56</v>
       </c>
-      <c r="E20" s="15" t="s">
-        <v>31</v>
+      <c r="E20" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="16">
+        <v>22</v>
+      </c>
+      <c r="G20" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17">
+      <c r="A21" s="16">
         <v>8</v>
       </c>
-      <c r="B21" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="28">
+      <c r="B21" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="25">
         <v>2.35</v>
       </c>
-      <c r="E21" s="21" t="s">
-        <v>31</v>
+      <c r="E21" s="19" t="s">
+        <v>28</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="22">
+        <v>22</v>
+      </c>
+      <c r="G21" s="20">
         <v>5</v>
       </c>
     </row>
@@ -2117,21 +2472,21 @@
         <v>9</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="14">
         <v>10</v>
       </c>
-      <c r="E22" s="15" t="s">
-        <v>31</v>
+      <c r="D22" s="26">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="16">
+        <v>20</v>
+      </c>
+      <c r="G22" s="15">
         <v>3</v>
       </c>
     </row>
@@ -2140,67 +2495,67 @@
         <v>9</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="14">
-        <v>4</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>31</v>
+        <v>11</v>
+      </c>
+      <c r="D23" s="26">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="16">
+        <v>20</v>
+      </c>
+      <c r="G23" s="15">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17">
+      <c r="A24" s="16">
         <v>9</v>
       </c>
-      <c r="B24" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="19" t="s">
+      <c r="B24" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="20">
-        <v>7</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>31</v>
+      <c r="C24" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="25">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>28</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="22">
+        <v>20</v>
+      </c>
+      <c r="G24" s="20">
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="23">
+      <c r="A25" s="21">
         <v>10</v>
       </c>
-      <c r="B25" s="24" t="s">
-        <v>19</v>
+      <c r="B25" s="22" t="s">
+        <v>16</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="25">
-        <v>4</v>
-      </c>
-      <c r="E25" s="26" t="s">
-        <v>31</v>
+        <v>10</v>
+      </c>
+      <c r="D25" s="27">
+        <v>4.55</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25" s="27">
+        <v>20</v>
+      </c>
+      <c r="G25" s="24">
         <v>6</v>
       </c>
     </row>
@@ -2209,67 +2564,67 @@
         <v>10</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="14">
-        <v>8</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>31</v>
+        <v>11</v>
+      </c>
+      <c r="D26" s="26">
+        <v>4.55</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="16">
+        <v>20</v>
+      </c>
+      <c r="G26" s="15">
         <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17">
+      <c r="A27" s="16">
         <v>10</v>
       </c>
-      <c r="B27" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="20">
+      <c r="B27" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="25">
+        <v>4.55</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="20">
         <v>6</v>
       </c>
-      <c r="E27" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" s="22">
-        <v>6</v>
-      </c>
     </row>
     <row r="28" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="23">
+      <c r="A28" s="21">
         <v>11</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="27">
+        <v>5.75</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="25">
-        <v>9</v>
-      </c>
-      <c r="E28" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G28" s="27">
+      <c r="G28" s="24">
         <v>7</v>
       </c>
     </row>
@@ -2278,67 +2633,67 @@
         <v>11</v>
       </c>
       <c r="B29" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="26">
+        <v>5.75</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="14">
-        <v>8</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" s="16">
+      <c r="G29" s="15">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="17">
+      <c r="A30" s="16">
         <v>11</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="25">
+        <v>5.75</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="20">
-        <v>8.5</v>
-      </c>
-      <c r="E30" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="22">
+      <c r="G30" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="23">
+      <c r="A31" s="21">
         <v>12</v>
       </c>
-      <c r="B31" s="24" t="s">
-        <v>21</v>
+      <c r="B31" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="25">
-        <v>2</v>
-      </c>
-      <c r="E31" s="26" t="s">
-        <v>31</v>
+        <v>10</v>
+      </c>
+      <c r="D31" s="27">
+        <v>6.8</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G31" s="27">
+        <v>20</v>
+      </c>
+      <c r="G31" s="24">
         <v>8</v>
       </c>
     </row>
@@ -2347,44 +2702,44 @@
         <v>12</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="14">
-        <v>1</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>31</v>
+        <v>11</v>
+      </c>
+      <c r="D32" s="26">
+        <v>6.8</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G32" s="16">
+        <v>20</v>
+      </c>
+      <c r="G32" s="15">
         <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="17">
+      <c r="A33" s="16">
         <v>12</v>
       </c>
-      <c r="B33" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33" s="20">
-        <v>2</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>31</v>
+      <c r="B33" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="25">
+        <v>6.8</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>28</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33" s="22">
+        <v>20</v>
+      </c>
+      <c r="G33" s="20">
         <v>8</v>
       </c>
     </row>
@@ -2392,22 +2747,22 @@
       <c r="A34" s="11">
         <v>13</v>
       </c>
-      <c r="B34" s="36" t="s">
-        <v>59</v>
+      <c r="B34" s="32" t="s">
+        <v>56</v>
       </c>
       <c r="C34" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D34">
         <v>7.8</v>
       </c>
-      <c r="E34" s="37" t="s">
-        <v>31</v>
+      <c r="E34" s="33" t="s">
+        <v>28</v>
       </c>
       <c r="F34" t="s">
-        <v>23</v>
-      </c>
-      <c r="G34" s="16">
+        <v>20</v>
+      </c>
+      <c r="G34" s="15">
         <v>8</v>
       </c>
     </row>
@@ -2415,22 +2770,22 @@
       <c r="A35" s="11">
         <v>14</v>
       </c>
-      <c r="B35" s="36" t="s">
-        <v>60</v>
+      <c r="B35" s="32" t="s">
+        <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D35">
         <v>5.9</v>
       </c>
-      <c r="E35" s="37" t="s">
-        <v>31</v>
+      <c r="E35" s="33" t="s">
+        <v>28</v>
       </c>
       <c r="F35" t="s">
-        <v>23</v>
-      </c>
-      <c r="G35" s="16">
+        <v>20</v>
+      </c>
+      <c r="G35" s="15">
         <v>8</v>
       </c>
     </row>
@@ -2438,45 +2793,45 @@
       <c r="A36" s="11">
         <v>15</v>
       </c>
-      <c r="B36" s="36" t="s">
-        <v>61</v>
+      <c r="B36" s="32" t="s">
+        <v>58</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D36">
         <v>1.75</v>
       </c>
-      <c r="E36" s="37" t="s">
-        <v>31</v>
+      <c r="E36" s="33" t="s">
+        <v>28</v>
       </c>
       <c r="F36" t="s">
-        <v>25</v>
-      </c>
-      <c r="G36" s="16">
+        <v>22</v>
+      </c>
+      <c r="G36" s="15">
         <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="23">
+      <c r="A37" s="21">
         <v>16</v>
       </c>
-      <c r="B37" s="35" t="s">
-        <v>62</v>
+      <c r="B37" s="31" t="s">
+        <v>59</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="25">
+        <v>10</v>
+      </c>
+      <c r="D37" s="27">
         <v>5.55</v>
       </c>
-      <c r="E37" s="26" t="s">
-        <v>31</v>
+      <c r="E37" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G37" s="27">
+        <v>66</v>
+      </c>
+      <c r="G37" s="24">
         <v>9</v>
       </c>
     </row>
@@ -2484,68 +2839,68 @@
       <c r="A38" s="11">
         <v>16</v>
       </c>
-      <c r="B38" s="36" t="s">
-        <v>62</v>
+      <c r="B38" s="32" t="s">
+        <v>59</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="38">
-        <v>5</v>
-      </c>
-      <c r="E38" s="37" t="s">
-        <v>31</v>
+        <v>11</v>
+      </c>
+      <c r="D38" s="41">
+        <v>5.55</v>
+      </c>
+      <c r="E38" s="33" t="s">
+        <v>28</v>
       </c>
       <c r="F38" t="s">
-        <v>69</v>
-      </c>
-      <c r="G38" s="16">
+        <v>66</v>
+      </c>
+      <c r="G38" s="15">
         <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="17">
+      <c r="A39" s="16">
         <v>16</v>
       </c>
-      <c r="B39" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" s="20">
-        <v>6.4</v>
-      </c>
-      <c r="E39" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F39" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="G39" s="22">
+      <c r="B39" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="25">
+        <v>5.55</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G39" s="20">
         <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="23">
+      <c r="A40" s="21">
         <v>17</v>
       </c>
-      <c r="B40" s="35" t="s">
-        <v>63</v>
+      <c r="B40" s="31" t="s">
+        <v>60</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D40" s="25">
-        <v>7.84</v>
-      </c>
-      <c r="E40" s="26" t="s">
-        <v>31</v>
+        <v>10</v>
+      </c>
+      <c r="D40" s="27">
+        <v>7.17</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G40" s="27">
+        <v>22</v>
+      </c>
+      <c r="G40" s="24">
         <v>9</v>
       </c>
     </row>
@@ -2553,68 +2908,68 @@
       <c r="A41" s="11">
         <v>17</v>
       </c>
-      <c r="B41" s="36" t="s">
-        <v>63</v>
+      <c r="B41" s="32" t="s">
+        <v>60</v>
       </c>
       <c r="C41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="38">
-        <v>5.85</v>
-      </c>
-      <c r="E41" s="37" t="s">
-        <v>31</v>
+        <v>11</v>
+      </c>
+      <c r="D41" s="41">
+        <v>7.17</v>
+      </c>
+      <c r="E41" s="33" t="s">
+        <v>28</v>
       </c>
       <c r="F41" t="s">
-        <v>25</v>
-      </c>
-      <c r="G41" s="16">
+        <v>22</v>
+      </c>
+      <c r="G41" s="15">
         <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="17">
+      <c r="A42" s="16">
         <v>17</v>
       </c>
-      <c r="B42" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D42" s="20">
+      <c r="B42" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="25">
         <v>7.17</v>
       </c>
-      <c r="E42" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F42" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G42" s="22">
+      <c r="E42" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" s="20">
         <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="23">
+      <c r="A43" s="21">
         <v>18</v>
       </c>
-      <c r="B43" s="35" t="s">
-        <v>64</v>
+      <c r="B43" s="31" t="s">
+        <v>61</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" s="25">
-        <v>9.6</v>
-      </c>
-      <c r="E43" s="26" t="s">
-        <v>31</v>
+        <v>10</v>
+      </c>
+      <c r="D43" s="27">
+        <v>7.8</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G43" s="27">
+        <v>20</v>
+      </c>
+      <c r="G43" s="24">
         <v>9</v>
       </c>
     </row>
@@ -2622,68 +2977,68 @@
       <c r="A44" s="11">
         <v>18</v>
       </c>
-      <c r="B44" s="36" t="s">
-        <v>64</v>
+      <c r="B44" s="32" t="s">
+        <v>61</v>
       </c>
       <c r="C44" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" s="38">
-        <v>6.5</v>
-      </c>
-      <c r="E44" s="37" t="s">
-        <v>31</v>
+        <v>11</v>
+      </c>
+      <c r="D44" s="41">
+        <v>7.8</v>
+      </c>
+      <c r="E44" s="33" t="s">
+        <v>28</v>
       </c>
       <c r="F44" t="s">
-        <v>23</v>
-      </c>
-      <c r="G44" s="16">
+        <v>20</v>
+      </c>
+      <c r="G44" s="15">
         <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="17">
+      <c r="A45" s="16">
         <v>18</v>
       </c>
-      <c r="B45" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D45" s="20">
+      <c r="B45" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" s="25">
         <v>7.8</v>
       </c>
-      <c r="E45" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F45" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="G45" s="22">
+      <c r="E45" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="20">
         <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="23">
+      <c r="A46" s="21">
         <v>19</v>
       </c>
-      <c r="B46" s="35" t="s">
-        <v>65</v>
+      <c r="B46" s="31" t="s">
+        <v>62</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46" s="25">
-        <v>5.76</v>
-      </c>
-      <c r="E46" s="26" t="s">
-        <v>31</v>
+        <v>10</v>
+      </c>
+      <c r="D46" s="27">
+        <v>5.19</v>
+      </c>
+      <c r="E46" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G46" s="27">
+        <v>66</v>
+      </c>
+      <c r="G46" s="24">
         <v>9</v>
       </c>
     </row>
@@ -2691,45 +3046,45 @@
       <c r="A47" s="11">
         <v>19</v>
       </c>
-      <c r="B47" s="36" t="s">
-        <v>65</v>
+      <c r="B47" s="32" t="s">
+        <v>62</v>
       </c>
       <c r="C47" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="38">
-        <v>3.74</v>
-      </c>
-      <c r="E47" s="37" t="s">
-        <v>31</v>
+        <v>11</v>
+      </c>
+      <c r="D47" s="41">
+        <v>5.19</v>
+      </c>
+      <c r="E47" s="33" t="s">
+        <v>28</v>
       </c>
       <c r="F47" t="s">
-        <v>69</v>
-      </c>
-      <c r="G47" s="16">
+        <v>66</v>
+      </c>
+      <c r="G47" s="15">
         <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="17">
+      <c r="A48" s="16">
         <v>19</v>
       </c>
-      <c r="B48" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="C48" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48" s="20">
-        <v>4.6399999999999997</v>
-      </c>
-      <c r="E48" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F48" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="G48" s="22">
+      <c r="B48" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="25">
+        <v>5.19</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F48" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G48" s="20">
         <v>9</v>
       </c>
     </row>
@@ -2737,45 +3092,45 @@
       <c r="A49" s="11">
         <v>20</v>
       </c>
-      <c r="B49" s="36" t="s">
-        <v>66</v>
+      <c r="B49" s="32" t="s">
+        <v>63</v>
       </c>
       <c r="C49" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D49">
         <v>5.43</v>
       </c>
-      <c r="E49" s="37" t="s">
-        <v>31</v>
+      <c r="E49" s="33" t="s">
+        <v>28</v>
       </c>
       <c r="F49" t="s">
-        <v>25</v>
-      </c>
-      <c r="G49" s="16">
+        <v>22</v>
+      </c>
+      <c r="G49" s="15">
         <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="23">
+      <c r="A50" s="21">
         <v>21</v>
       </c>
-      <c r="B50" s="35" t="s">
-        <v>67</v>
+      <c r="B50" s="31" t="s">
+        <v>64</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" s="25">
-        <v>5.2</v>
-      </c>
-      <c r="E50" s="26" t="s">
-        <v>31</v>
+        <v>10</v>
+      </c>
+      <c r="D50" s="27">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E50" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G50" s="27">
+        <v>20</v>
+      </c>
+      <c r="G50" s="24">
         <v>10</v>
       </c>
     </row>
@@ -2783,45 +3138,45 @@
       <c r="A51" s="11">
         <v>21</v>
       </c>
-      <c r="B51" s="36" t="s">
-        <v>67</v>
+      <c r="B51" s="32" t="s">
+        <v>64</v>
       </c>
       <c r="C51" t="s">
-        <v>14</v>
-      </c>
-      <c r="D51" s="38">
-        <v>2.1</v>
-      </c>
-      <c r="E51" s="37" t="s">
-        <v>31</v>
+        <v>11</v>
+      </c>
+      <c r="D51" s="41">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E51" s="33" t="s">
+        <v>28</v>
       </c>
       <c r="F51" t="s">
-        <v>23</v>
-      </c>
-      <c r="G51" s="16">
+        <v>20</v>
+      </c>
+      <c r="G51" s="15">
         <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="17">
+      <c r="A52" s="16">
         <v>21</v>
       </c>
-      <c r="B52" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="C52" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D52" s="20">
-        <v>3.4</v>
-      </c>
-      <c r="E52" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F52" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="G52" s="22">
+      <c r="B52" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" s="25">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E52" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F52" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G52" s="20">
         <v>10</v>
       </c>
     </row>
@@ -2829,22 +3184,22 @@
       <c r="A53" s="11">
         <v>22</v>
       </c>
-      <c r="B53" s="36" t="s">
-        <v>68</v>
+      <c r="B53" s="32" t="s">
+        <v>65</v>
       </c>
       <c r="C53" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D53">
         <v>5</v>
       </c>
-      <c r="E53" s="37" t="s">
-        <v>31</v>
+      <c r="E53" s="33" t="s">
+        <v>28</v>
       </c>
       <c r="F53" t="s">
-        <v>25</v>
-      </c>
-      <c r="G53" s="16">
+        <v>22</v>
+      </c>
+      <c r="G53" s="15">
         <v>10</v>
       </c>
     </row>
@@ -2867,14 +3222,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="38" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2882,7 +3237,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -2893,7 +3248,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -2904,7 +3259,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2915,7 +3270,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -2926,7 +3281,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -2937,7 +3292,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -2948,7 +3303,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -2959,7 +3314,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -2970,7 +3325,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -2981,7 +3336,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -2992,7 +3347,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -3003,7 +3358,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -3013,8 +3368,8 @@
       <c r="A14" s="13">
         <v>13</v>
       </c>
-      <c r="B14" s="44" t="s">
-        <v>59</v>
+      <c r="B14" s="39" t="s">
+        <v>56</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -3024,8 +3379,8 @@
       <c r="A15" s="13">
         <v>14</v>
       </c>
-      <c r="B15" s="44" t="s">
-        <v>60</v>
+      <c r="B15" s="39" t="s">
+        <v>57</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -3035,8 +3390,8 @@
       <c r="A16" s="13">
         <v>15</v>
       </c>
-      <c r="B16" s="44" t="s">
-        <v>61</v>
+      <c r="B16" s="39" t="s">
+        <v>58</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -3046,8 +3401,8 @@
       <c r="A17" s="13">
         <v>16</v>
       </c>
-      <c r="B17" s="44" t="s">
-        <v>62</v>
+      <c r="B17" s="39" t="s">
+        <v>59</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -3057,8 +3412,8 @@
       <c r="A18" s="13">
         <v>17</v>
       </c>
-      <c r="B18" s="44" t="s">
-        <v>63</v>
+      <c r="B18" s="39" t="s">
+        <v>60</v>
       </c>
       <c r="C18">
         <v>4</v>
@@ -3068,8 +3423,8 @@
       <c r="A19" s="13">
         <v>18</v>
       </c>
-      <c r="B19" s="44" t="s">
-        <v>64</v>
+      <c r="B19" s="39" t="s">
+        <v>61</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -3079,8 +3434,8 @@
       <c r="A20" s="13">
         <v>19</v>
       </c>
-      <c r="B20" s="44" t="s">
-        <v>65</v>
+      <c r="B20" s="39" t="s">
+        <v>62</v>
       </c>
       <c r="C20">
         <v>3</v>
@@ -3090,8 +3445,8 @@
       <c r="A21" s="13">
         <v>20</v>
       </c>
-      <c r="B21" s="44" t="s">
-        <v>66</v>
+      <c r="B21" s="39" t="s">
+        <v>63</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -3101,8 +3456,8 @@
       <c r="A22" s="13">
         <v>21</v>
       </c>
-      <c r="B22" s="44" t="s">
-        <v>67</v>
+      <c r="B22" s="39" t="s">
+        <v>64</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -3112,8 +3467,8 @@
       <c r="A23" s="11">
         <v>22</v>
       </c>
-      <c r="B23" s="36" t="s">
-        <v>68</v>
+      <c r="B23" s="32" t="s">
+        <v>65</v>
       </c>
       <c r="C23">
         <v>4</v>
@@ -3141,55 +3496,55 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
-        <v>69</v>
+      <c r="A2" s="35" t="s">
+        <v>66</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
-        <v>69</v>
+      <c r="A3" s="35" t="s">
+        <v>66</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D3">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
-        <v>69</v>
+      <c r="A4" s="35" t="s">
+        <v>66</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -3197,13 +3552,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -3211,13 +3566,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>3.33</v>
@@ -3225,13 +3580,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D7">
         <v>6.66</v>
@@ -3239,13 +3594,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -3253,13 +3608,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -3267,13 +3622,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>2.5</v>
@@ -3281,13 +3636,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -3295,13 +3650,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B12">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D12">
         <v>7.5</v>
@@ -3309,13 +3664,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B13">
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -3323,13 +3678,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D14">
         <v>10</v>
@@ -3337,13 +3692,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -3351,13 +3706,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>99</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -3380,16 +3735,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
-        <v>22</v>
+      <c r="A1" s="37" t="s">
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
-        <v>69</v>
+      <c r="A2" s="35" t="s">
+        <v>66</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -3397,15 +3752,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
-        <v>26</v>
+      <c r="A4" s="35" t="s">
+        <v>23</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -3413,15 +3768,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
-        <v>27</v>
+      <c r="A6" s="35" t="s">
+        <v>24</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3435,10 +3790,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5054A09C-27DF-A543-9E5F-5391BB5AD097}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3448,14 +3803,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="28" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3466,7 +3821,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3477,7 +3832,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3488,40 +3843,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
         <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -3543,11 +3865,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
-        <v>52</v>
+      <c r="A1" s="30" t="s">
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -3555,7 +3877,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3563,7 +3885,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -3571,7 +3893,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -3579,7 +3901,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -3587,7 +3909,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3595,7 +3917,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -3603,7 +3925,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3611,7 +3933,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -3619,7 +3941,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -3627,7 +3949,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>